<commit_message>
mise a jour des données
</commit_message>
<xml_diff>
--- a/data/donneesCorona.xlsx
+++ b/data/donneesCorona.xlsx
@@ -1873,7 +1873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0" zoomScale="108">
       <selection activeCell="L35" sqref="L35"/>
@@ -2030,6 +2030,34 @@
         <v>12</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" s="9" t="n">
+        <v>43912.69236697095</v>
+      </c>
+      <c r="B15" t="n">
+        <v>14485</v>
+      </c>
+      <c r="C15" t="n">
+        <v>562</v>
+      </c>
+      <c r="D15" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9" t="n">
+        <v>43912.76475450717</v>
+      </c>
+      <c r="B16" t="n">
+        <v>14485</v>
+      </c>
+      <c r="C16" t="n">
+        <v>562</v>
+      </c>
+      <c r="D16" t="n">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:M1"/>
@@ -2045,7 +2073,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="107">
       <selection activeCell="A5" sqref="A5"/>
@@ -2191,6 +2219,34 @@
         <v>93790</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" s="9" t="n">
+        <v>43912.69236697095</v>
+      </c>
+      <c r="B10" t="n">
+        <v>316652</v>
+      </c>
+      <c r="C10" t="n">
+        <v>13598</v>
+      </c>
+      <c r="D10" t="n">
+        <v>94176</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="9" t="n">
+        <v>43912.76475450717</v>
+      </c>
+      <c r="B11" t="n">
+        <v>318662</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13672</v>
+      </c>
+      <c r="D11" t="n">
+        <v>94704</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2202,7 +2258,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
       <selection activeCell="D12" sqref="D12"/>
@@ -3048,6 +3104,234 @@
         <v>90.93000000000001</v>
       </c>
     </row>
+    <row r="47">
+      <c r="A47" s="9" t="n">
+        <v>43912.69242277653</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>4.57</v>
+      </c>
+      <c r="D47" t="n">
+        <v>4.13</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="9" t="n">
+        <v>43912.69242277653</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Italie</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>16.92</v>
+      </c>
+      <c r="D48" t="n">
+        <v>35.48</v>
+      </c>
+      <c r="E48" t="n">
+        <v>6.45</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="9" t="n">
+        <v>43912.69242277653</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Espagne</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>9.02</v>
+      </c>
+      <c r="D49" t="n">
+        <v>12.65</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2.26</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="9" t="n">
+        <v>43912.69242277653</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Allemagne</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>7.55</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.68</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="9" t="n">
+        <v>43912.69242277653</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="D51" t="n">
+        <v>1.72</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="9" t="n">
+        <v>43912.69242277653</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Reste du monde</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>60.34</v>
+      </c>
+      <c r="D52" t="n">
+        <v>45.34</v>
+      </c>
+      <c r="E52" t="n">
+        <v>90.93000000000001</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="9" t="n">
+        <v>43912.76479431608</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>4.55</v>
+      </c>
+      <c r="D53" t="n">
+        <v>4.11</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="9" t="n">
+        <v>43912.76479431608</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Italie</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>16.81</v>
+      </c>
+      <c r="D54" t="n">
+        <v>35.29</v>
+      </c>
+      <c r="E54" t="n">
+        <v>6.41</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="9" t="n">
+        <v>43912.76479431608</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Espagne</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>8.98</v>
+      </c>
+      <c r="D55" t="n">
+        <v>12.84</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2.72</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="9" t="n">
+        <v>43912.76479431608</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Allemagne</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>7.52</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.28</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="9" t="n">
+        <v>43912.76479431608</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="D57" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="9" t="n">
+        <v>43912.76479431608</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Reste du monde</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>60.55</v>
+      </c>
+      <c r="D58" t="n">
+        <v>45.38</v>
+      </c>
+      <c r="E58" t="n">
+        <v>90.51000000000001</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
mise a jour des donnees
</commit_message>
<xml_diff>
--- a/data/donneesCorona.xlsx
+++ b/data/donneesCorona.xlsx
@@ -1873,7 +1873,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M16"/>
+  <dimension ref="A1:M17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0" zoomScale="108">
       <selection activeCell="L35" sqref="L35"/>
@@ -2058,6 +2058,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="17">
+      <c r="A17" s="9" t="n">
+        <v>43913.81262007809</v>
+      </c>
+      <c r="B17" t="n">
+        <v>16937</v>
+      </c>
+      <c r="C17" t="n">
+        <v>676</v>
+      </c>
+      <c r="D17" t="n">
+        <v>2207</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G1:M1"/>
@@ -2073,7 +2087,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="107">
       <selection activeCell="A5" sqref="A5"/>
@@ -2247,6 +2261,20 @@
         <v>94704</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" s="9" t="n">
+        <v>43913.81262007809</v>
+      </c>
+      <c r="B12" t="n">
+        <v>367457</v>
+      </c>
+      <c r="C12" t="n">
+        <v>16113</v>
+      </c>
+      <c r="D12" t="n">
+        <v>100879</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -2258,7 +2286,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A33" workbookViewId="0" zoomScale="110" zoomScaleNormal="110">
       <selection activeCell="D12" sqref="D12"/>
@@ -3332,6 +3360,120 @@
         <v>90.51000000000001</v>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" s="9" t="n">
+        <v>43913.81266451103</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>France</t>
+        </is>
+      </c>
+      <c r="C59" t="n">
+        <v>4.61</v>
+      </c>
+      <c r="D59" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="E59" t="n">
+        <v>2.19</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="9" t="n">
+        <v>43913.81266451103</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Italie</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>17.4</v>
+      </c>
+      <c r="D60" t="n">
+        <v>37.71</v>
+      </c>
+      <c r="E60" t="n">
+        <v>7.37</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="9" t="n">
+        <v>43913.81266451103</v>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Espagne</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>9</v>
+      </c>
+      <c r="D61" t="n">
+        <v>13.69</v>
+      </c>
+      <c r="E61" t="n">
+        <v>3.33</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="9" t="n">
+        <v>43913.81266451103</v>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>Allemagne</t>
+        </is>
+      </c>
+      <c r="C62" t="n">
+        <v>7.86</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.73</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.42</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="9" t="n">
+        <v>43913.81266451103</v>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>UK</t>
+        </is>
+      </c>
+      <c r="C63" t="n">
+        <v>1.61</v>
+      </c>
+      <c r="D63" t="n">
+        <v>2.09</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="9" t="n">
+        <v>43913.81266451103</v>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>Reste du monde</t>
+        </is>
+      </c>
+      <c r="C64" t="n">
+        <v>59.52</v>
+      </c>
+      <c r="D64" t="n">
+        <v>41.58</v>
+      </c>
+      <c r="E64" t="n">
+        <v>86.55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>